<commit_message>
included new dump with criteria catalog showing betroffenenrechte
</commit_message>
<xml_diff>
--- a/webcentral/doc/01_data/08_criteria_catalog/criteria_catalog_betriebsoptimierung_20240916.xlsx
+++ b/webcentral/doc/01_data/08_criteria_catalog/criteria_catalog_betriebsoptimierung_20240916.xlsx
@@ -2535,7 +2535,7 @@
 - https://www.datenschutz-mv.de/static/DS/Dateien/Entschliessungen/Datenschutz/20210315_Beschluss_Energieversorgerpool.pdf</t>
   </si>
   <si>
-    <t xml:space="preserve">topic_XV.svg</t>
+    <t xml:space="preserve">topic_literature.svg</t>
   </si>
   <si>
     <t xml:space="preserve">True</t>
@@ -3063,8 +3063,8 @@
   </sheetPr>
   <dimension ref="A1:Z1208"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A133" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M160" activeCellId="0" sqref="M160"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A190" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F210" activeCellId="0" sqref="F210"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.66796875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>